<commit_message>
Esercizi: 1 e 2
</commit_message>
<xml_diff>
--- a/ESERCIZIO 2.xlsx
+++ b/ESERCIZIO 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salvo/Desktop/Epicode esercizi/Esercizi del 12:12:23/M2-1-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292479A6-8356-044D-A689-A2B2C04BD966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18D784A-D215-8242-9C3A-D30A0D09AEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="500" windowWidth="27940" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Assoluti_Iva!$A$4:$C$340</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CONTA!$A$1:$A$110</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">LOGICA!$A$1:$D$80</definedName>
     <definedName name="abitanti">CONTA!$B$2:$B$110</definedName>
     <definedName name="ACCES">Assoluti_Iva!$A$196:$C$230</definedName>
@@ -921,7 +922,7 @@
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -947,7 +948,6 @@
     <xf numFmtId="168" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1289,7 +1289,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1306,18 +1306,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="102.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>193</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>184</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
       <c r="G3" s="13" t="s">
         <v>205</v>
       </c>
@@ -1341,7 +1341,7 @@
       <c r="F4" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="28">
         <f>SUM(C5:C340,)</f>
         <v>171416000</v>
       </c>
@@ -1353,7 +1353,7 @@
       <c r="A5" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="28"/>
+      <c r="B5" s="27"/>
       <c r="C5" s="9">
         <v>281000</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>323000</v>
       </c>
       <c r="D6" s="7" t="str">
-        <f t="shared" ref="D5:D69" si="0">IF(AND(B6="Abbigliamento", C6&gt;300000), "TROVATO", "")</f>
+        <f t="shared" ref="D6:D69" si="0">IF(AND(B6="Abbigliamento", C6&gt;300000), "TROVATO", "")</f>
         <v>TROVATO</v>
       </c>
       <c r="E6" s="7" t="str">
@@ -1496,7 +1496,7 @@
       <c r="A11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="9">
@@ -1565,7 +1565,7 @@
       <c r="A14" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="9">
@@ -3313,7 +3313,7 @@
       <c r="A90" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B90" s="30" t="s">
+      <c r="B90" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C90" s="9">
@@ -3382,7 +3382,7 @@
       <c r="A93" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B93" s="30" t="s">
+      <c r="B93" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C93" s="9">
@@ -5128,7 +5128,7 @@
       <c r="A169" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B169" s="30" t="s">
+      <c r="B169" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C169" s="9">
@@ -5197,7 +5197,7 @@
       <c r="A172" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B172" s="30" t="s">
+      <c r="B172" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C172" s="9">
@@ -6939,7 +6939,7 @@
       <c r="A248" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B248" s="30" t="s">
+      <c r="B248" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C248" s="9">
@@ -7008,7 +7008,7 @@
       <c r="A251" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B251" s="30" t="s">
+      <c r="B251" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C251" s="9">
@@ -8752,7 +8752,7 @@
       <c r="A327" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B327" s="30" t="s">
+      <c r="B327" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C327" s="9">
@@ -8821,7 +8821,7 @@
       <c r="A330" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B330" s="30" t="s">
+      <c r="B330" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C330" s="9">
@@ -9098,7 +9098,7 @@
   <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9169,7 +9169,10 @@
       <c r="G3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="22"/>
+      <c r="H3" s="22">
+        <f>SUMIF(cate,G3,import)</f>
+        <v>611780</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -9190,7 +9193,10 @@
       <c r="G4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="H4" s="22"/>
+      <c r="H4" s="22">
+        <f>SUMIF(cate,G4,import)</f>
+        <v>30860</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -9211,7 +9217,10 @@
       <c r="G5" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="22"/>
+      <c r="H5" s="22">
+        <f>SUMIF(cate,G5,import)</f>
+        <v>54000</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -9232,7 +9241,10 @@
       <c r="G6" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="H6" s="22"/>
+      <c r="H6" s="22">
+        <f>SUMIF(cate,G6,import)</f>
+        <v>6765600</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
@@ -9251,7 +9263,7 @@
         <v>22</v>
       </c>
       <c r="G7" s="18"/>
-      <c r="H7" s="25"/>
+      <c r="H7" s="22"/>
     </row>
     <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -9272,7 +9284,10 @@
       <c r="G8" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="22">
+        <f>SUMIF(clie,G8,import)</f>
+        <v>73450</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -9293,7 +9308,10 @@
       <c r="G9" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="22"/>
+      <c r="H9" s="22">
+        <f>SUMIF(clie,G9,import)</f>
+        <v>50800</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -9314,7 +9332,10 @@
       <c r="G10" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="22"/>
+      <c r="H10" s="22">
+        <f>SUMIF(clie,G10,import)</f>
+        <v>98450</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -9335,7 +9356,10 @@
       <c r="G11" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="22"/>
+      <c r="H11" s="22">
+        <f>SUMIF(clie,G11,import)</f>
+        <v>7950</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -9356,7 +9380,10 @@
       <c r="G12" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="H12" s="22"/>
+      <c r="H12" s="22">
+        <f>SUMIF(clie,G12,import)</f>
+        <v>283000</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -9377,7 +9404,10 @@
       <c r="G13" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="22"/>
+      <c r="H13" s="22">
+        <f>SUMIF(clie,G13,import)</f>
+        <v>107700</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -9398,7 +9428,10 @@
       <c r="G14" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="H14" s="22"/>
+      <c r="H14" s="22">
+        <f>SUMIF(clie,G14,import)</f>
+        <v>27270</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="2">
@@ -10542,7 +10575,7 @@
   <dimension ref="A1:E110"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -10569,14 +10602,20 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="25" t="s">
         <v>130</v>
       </c>
       <c r="B2" s="24">
         <v>125</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="D2" s="23">
+        <f>SUMIF(A:A,"OSSENIGO",B:B)</f>
+        <v>130</v>
+      </c>
+      <c r="E2" s="23">
+        <f>SUMIF(A:A,"AVIO",B:B)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
@@ -10604,7 +10643,10 @@
       <c r="B5" s="24">
         <v>5</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="26">
+        <f>COUNTIF(B:B,"&gt;100")</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A6" s="24" t="s">
@@ -10624,6 +10666,10 @@
       <c r="B7" s="24">
         <v>75</v>
       </c>
+      <c r="D7">
+        <f>COUNTIF(A2:A110,"C*")</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="24" t="s">
@@ -10643,6 +10689,10 @@
       <c r="B9" s="24">
         <v>5</v>
       </c>
+      <c r="D9">
+        <f>COUNTIFS(B:B,"&gt;10",B:B,"&lt;100")</f>
+        <v>47</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A10" s="24" t="s">
@@ -10662,6 +10712,10 @@
       <c r="B11" s="24">
         <v>29</v>
       </c>
+      <c r="D11">
+        <f>SUM(B:B)</f>
+        <v>12564</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A12" s="24" t="s">
@@ -11456,6 +11510,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A110" xr:uid="{5CBD8C3F-135D-4280-BD95-8C23E6C981DD}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>